<commit_message>
v1.0.8 Character Ability Update
</commit_message>
<xml_diff>
--- a/rand-pokemon%.xlsx
+++ b/rand-pokemon%.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mm\PycharmProjects\Pokemon Arena\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768566C9-8858-40AF-9C64-3D6CD8A956D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3E65DE-5D69-415F-B468-016802ED611A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BBCBD22B-4CDD-4B10-9645-627E2745DCA9}"/>
   </bookViews>
@@ -456,13 +456,13 @@
   <dimension ref="A1:N203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R37" sqref="R37"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="7" width="9.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="2" max="7" width="9.140625" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" hidden="1" customWidth="1"/>
     <col min="9" max="13" width="9.140625" style="1"/>
   </cols>
   <sheetData>

</xml_diff>